<commit_message>
Update DA of metabolome data MetaboDiff columns organized and correct HMDB 3.xlsx
</commit_message>
<xml_diff>
--- a/MetaboDiff metabolome data/MetaboDiff Results/DA of metabolome data MetaboDiff columns organized and correct HMDB 3.xlsx
+++ b/MetaboDiff metabolome data/MetaboDiff Results/DA of metabolome data MetaboDiff columns organized and correct HMDB 3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/34420f5773a88cdb/Documents/UM documents/BMS Year 3/Internship ^M Thesis/Sabrina_BMS_Bachelor-Internship/MetaboDiff metabolome data/MetaboDiff Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:40009_{F4FFD494-5004-4FB9-8A43-9A27079081D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8CE6F0E2-7B2A-41B7-BD3C-016A830F08F7}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:40009_{F4FFD494-5004-4FB9-8A43-9A27079081D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5532CC2D-DCAE-4976-B852-B999CE5733BA}"/>
   <bookViews>
-    <workbookView xWindow="9630" yWindow="0" windowWidth="9730" windowHeight="9740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8740" yWindow="70" windowWidth="10420" windowHeight="10150" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DA of metabolome data MetaboDif" sheetId="1" r:id="rId1"/>
@@ -1835,8 +1835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D324"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6394,8 +6394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5540763-C8AF-4572-A154-2032FBC0CCE5}">
   <dimension ref="A1:D324"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7844,8 +7844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F33B6004-2F78-4F3A-8D17-183528C3609F}">
   <dimension ref="A1:D324"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D8"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7868,169 +7868,169 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="17">
         <v>-1.33607842980957</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="18">
         <v>3.2818247813940399E-5</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="17">
         <v>5.3001470219513798E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" s="8">
+        <v>-1.0997733070167699</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1.72634793125746E-2</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0.28069102837216803</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="B4" s="17">
+        <v>-1.0893286271079801</v>
+      </c>
+      <c r="C4" s="17">
+        <v>9.1921687118985999E-4</v>
+      </c>
+      <c r="D4" s="17">
+        <v>4.2415292770617799E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="17">
+        <v>-0.79500138609436999</v>
+      </c>
+      <c r="C5" s="17">
+        <v>7.3436061721981105E-4</v>
+      </c>
+      <c r="D5" s="17">
+        <v>3.9533079893666501E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B6" s="17">
         <v>-0.75760165598269003</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C6" s="18">
         <v>2.0049727023092699E-5</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D6" s="17">
         <v>5.3001470219513798E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="B4" s="11">
-        <v>0.21240903417253801</v>
-      </c>
-      <c r="C4" s="11">
-        <v>2.1006699903141401E-4</v>
-      </c>
-      <c r="D4" s="11">
-        <v>2.2617213562382301E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
+    <row r="7" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="8">
+        <v>-0.72013620780779797</v>
+      </c>
+      <c r="C7" s="8">
+        <v>8.5211976749304304E-3</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.161902755823678</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B8" s="17">
         <v>-0.68311383205169596</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C8" s="17">
         <v>4.0702678799256302E-4</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D8" s="17">
         <v>2.6483540458081999E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="8">
-        <v>-0.32735275573360001</v>
-      </c>
-      <c r="C6" s="8">
-        <v>4.0996192659569598E-4</v>
-      </c>
-      <c r="D6" s="8">
-        <v>2.6483540458081999E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B7" s="8">
-        <v>-0.79500138609436999</v>
-      </c>
-      <c r="C7" s="8">
-        <v>7.3436061721981105E-4</v>
-      </c>
-      <c r="D7" s="8">
-        <v>3.9533079893666501E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="B8" s="8">
-        <v>-1.0893286271079801</v>
-      </c>
-      <c r="C8" s="8">
-        <v>9.1921687118985999E-4</v>
-      </c>
-      <c r="D8" s="8">
-        <v>4.2415292770617799E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>261</v>
+        <v>202</v>
       </c>
       <c r="B9" s="8">
-        <v>-0.33171206325200803</v>
+        <v>-0.59076056723477099</v>
       </c>
       <c r="C9" s="8">
-        <v>1.3380775082738399E-3</v>
+        <v>7.23897702046043E-3</v>
       </c>
       <c r="D9" s="8">
-        <v>5.4024879396556202E-2</v>
+        <v>0.157671563728815</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="11">
-        <v>0.198056698819602</v>
-      </c>
-      <c r="C10" s="11">
-        <v>2.8758871486911498E-3</v>
-      </c>
-      <c r="D10" s="11">
-        <v>0.10321239433635999</v>
+      <c r="A10" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="B10" s="8">
+        <v>-0.552672333486111</v>
+      </c>
+      <c r="C10" s="8">
+        <v>2.2268252558053699E-2</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.32623070856498299</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="11">
-        <v>0.60368195934063695</v>
-      </c>
-      <c r="C11" s="11">
-        <v>3.28809754458113E-3</v>
-      </c>
-      <c r="D11" s="11">
-        <v>0.10620555068997101</v>
+      <c r="A11" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="B11" s="8">
+        <v>-0.48452756496974903</v>
+      </c>
+      <c r="C11" s="8">
+        <v>6.1874585908605903E-3</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.157671563728815</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
-        <v>202</v>
+        <v>126</v>
       </c>
       <c r="B12" s="8">
-        <v>-0.59076056723477099</v>
+        <v>-0.42477578132881899</v>
       </c>
       <c r="C12" s="8">
-        <v>7.23897702046043E-3</v>
+        <v>4.8658691314383697E-2</v>
       </c>
       <c r="D12" s="8">
-        <v>0.157671563728815</v>
+        <v>0.39743771373710102</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="B13" s="8">
-        <v>-0.48452756496974903</v>
+        <v>-0.39546690427175002</v>
       </c>
       <c r="C13" s="8">
-        <v>6.1874585908605903E-3</v>
+        <v>6.6455994836238201E-3</v>
       </c>
       <c r="D13" s="8">
         <v>0.157671563728815</v>
@@ -8038,55 +8038,55 @@
     </row>
     <row r="14" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
-        <v>185</v>
+        <v>101</v>
       </c>
       <c r="B14" s="8">
-        <v>-0.39546690427175002</v>
+        <v>-0.35997498978816</v>
       </c>
       <c r="C14" s="8">
-        <v>6.6455994836238201E-3</v>
+        <v>2.7271199497044402E-2</v>
       </c>
       <c r="D14" s="8">
-        <v>0.157671563728815</v>
+        <v>0.32623070856498299</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="11">
-        <v>0.128924160086271</v>
-      </c>
-      <c r="C15" s="11">
-        <v>7.3222088418954103E-3</v>
-      </c>
-      <c r="D15" s="11">
-        <v>0.157671563728815</v>
+      <c r="A15" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="B15" s="8">
+        <v>-0.33171206325200803</v>
+      </c>
+      <c r="C15" s="8">
+        <v>1.3380775082738399E-3</v>
+      </c>
+      <c r="D15" s="8">
+        <v>5.4024879396556202E-2</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="B16" s="11">
-        <v>0.40876233409423801</v>
-      </c>
-      <c r="C16" s="11">
-        <v>7.2453229715699098E-3</v>
-      </c>
-      <c r="D16" s="11">
-        <v>0.157671563728815</v>
+      <c r="A16" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="17">
+        <v>-0.32735275573360001</v>
+      </c>
+      <c r="C16" s="17">
+        <v>4.0996192659569598E-4</v>
+      </c>
+      <c r="D16" s="17">
+        <v>2.6483540458081999E-2</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="B17" s="8">
-        <v>-0.72013620780779797</v>
+        <v>-0.31258282366021101</v>
       </c>
       <c r="C17" s="8">
-        <v>8.5211976749304304E-3</v>
+        <v>8.4231301171404805E-3</v>
       </c>
       <c r="D17" s="8">
         <v>0.161902755823678</v>
@@ -8094,153 +8094,153 @@
     </row>
     <row r="18" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
-        <v>32</v>
+        <v>203</v>
       </c>
       <c r="B18" s="8">
-        <v>-0.31258282366021101</v>
+        <v>-0.26936200946180999</v>
       </c>
       <c r="C18" s="8">
-        <v>8.4231301171404805E-3</v>
+        <v>3.3973193460251801E-2</v>
       </c>
       <c r="D18" s="8">
-        <v>0.161902755823678</v>
+        <v>0.32623070856498299</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
-        <v>194</v>
+        <v>235</v>
       </c>
       <c r="B19" s="8">
-        <v>-1.0997733070167699</v>
+        <v>-0.19898487085320901</v>
       </c>
       <c r="C19" s="8">
-        <v>1.72634793125746E-2</v>
+        <v>2.7392105990339501E-2</v>
       </c>
       <c r="D19" s="8">
-        <v>0.28069102837216803</v>
+        <v>0.32623070856498299</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="B20" s="8">
-        <v>-0.115109238467447</v>
+        <v>-0.161461666507979</v>
       </c>
       <c r="C20" s="8">
-        <v>1.6538729190785199E-2</v>
+        <v>2.0757649109206001E-2</v>
       </c>
       <c r="D20" s="8">
-        <v>0.28069102837216803</v>
+        <v>0.31927241248921601</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="11">
-        <v>0.16512944122377199</v>
-      </c>
-      <c r="C21" s="11">
-        <v>1.7380249434809199E-2</v>
-      </c>
-      <c r="D21" s="11">
-        <v>0.28069102837216803</v>
+      <c r="A21" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B21" s="8">
+        <v>-0.15467735030756199</v>
+      </c>
+      <c r="C21" s="8">
+        <v>2.7232243139578699E-2</v>
+      </c>
+      <c r="D21" s="8">
+        <v>0.32623070856498299</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
-        <v>59</v>
+        <v>96</v>
       </c>
       <c r="B22" s="8">
-        <v>-0.161461666507979</v>
+        <v>-0.115109238467447</v>
       </c>
       <c r="C22" s="8">
-        <v>2.0757649109206001E-2</v>
+        <v>1.6538729190785199E-2</v>
       </c>
       <c r="D22" s="8">
-        <v>0.31927241248921601</v>
+        <v>0.28069102837216803</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="B23" s="8">
-        <v>-0.552672333486111</v>
-      </c>
-      <c r="C23" s="8">
-        <v>2.2268252558053699E-2</v>
-      </c>
-      <c r="D23" s="8">
+      <c r="A23" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="B23" s="11">
+        <v>0.103822849978464</v>
+      </c>
+      <c r="C23" s="11">
+        <v>3.4321705138369997E-2</v>
+      </c>
+      <c r="D23" s="11">
         <v>0.32623070856498299</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="B24" s="8">
-        <v>-0.35997498978816</v>
-      </c>
-      <c r="C24" s="8">
-        <v>2.7271199497044402E-2</v>
-      </c>
-      <c r="D24" s="8">
+      <c r="A24" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="11">
+        <v>0.128924160086271</v>
+      </c>
+      <c r="C24" s="11">
+        <v>7.3222088418954103E-3</v>
+      </c>
+      <c r="D24" s="11">
+        <v>0.157671563728815</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="11">
+        <v>0.144981570892874</v>
+      </c>
+      <c r="C25" s="11">
+        <v>3.0241915444754498E-2</v>
+      </c>
+      <c r="D25" s="11">
         <v>0.32623070856498299</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="B25" s="8">
-        <v>-0.26936200946180999</v>
-      </c>
-      <c r="C25" s="8">
-        <v>3.3973193460251801E-2</v>
-      </c>
-      <c r="D25" s="8">
+    <row r="26" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="11">
+        <v>0.14593478977736399</v>
+      </c>
+      <c r="C26" s="11">
+        <v>2.6384324377656899E-2</v>
+      </c>
+      <c r="D26" s="11">
         <v>0.32623070856498299</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="B26" s="8">
-        <v>-0.19898487085320901</v>
-      </c>
-      <c r="C26" s="8">
-        <v>2.7392105990339501E-2</v>
-      </c>
-      <c r="D26" s="8">
-        <v>0.32623070856498299</v>
-      </c>
-    </row>
     <row r="27" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="B27" s="8">
-        <v>-0.15467735030756199</v>
-      </c>
-      <c r="C27" s="8">
-        <v>2.7232243139578699E-2</v>
-      </c>
-      <c r="D27" s="8">
+      <c r="A27" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="11">
+        <v>0.15721786948573099</v>
+      </c>
+      <c r="C27" s="11">
+        <v>3.46889817874695E-2</v>
+      </c>
+      <c r="D27" s="11">
         <v>0.32623070856498299</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
-        <v>252</v>
+        <v>223</v>
       </c>
       <c r="B28" s="11">
-        <v>0.103822849978464</v>
+        <v>0.16274006457565099</v>
       </c>
       <c r="C28" s="11">
-        <v>3.4321705138369997E-2</v>
+        <v>3.6876426191857499E-2</v>
       </c>
       <c r="D28" s="11">
         <v>0.32623070856498299</v>
@@ -8248,27 +8248,27 @@
     </row>
     <row r="29" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="B29" s="11">
-        <v>0.144981570892874</v>
+        <v>0.16512944122377199</v>
       </c>
       <c r="C29" s="11">
-        <v>3.0241915444754498E-2</v>
+        <v>1.7380249434809199E-2</v>
       </c>
       <c r="D29" s="11">
-        <v>0.32623070856498299</v>
+        <v>0.28069102837216803</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="s">
-        <v>48</v>
+        <v>250</v>
       </c>
       <c r="B30" s="11">
-        <v>0.14593478977736399</v>
+        <v>0.17201846527610301</v>
       </c>
       <c r="C30" s="11">
-        <v>2.6384324377656899E-2</v>
+        <v>3.5586675930752001E-2</v>
       </c>
       <c r="D30" s="11">
         <v>0.32623070856498299</v>
@@ -8276,44 +8276,44 @@
     </row>
     <row r="31" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
-        <v>43</v>
+        <v>247</v>
       </c>
       <c r="B31" s="11">
-        <v>0.15721786948573099</v>
+        <v>0.18582779031259</v>
       </c>
       <c r="C31" s="11">
-        <v>3.46889817874695E-2</v>
+        <v>4.9218292722860803E-2</v>
       </c>
       <c r="D31" s="11">
-        <v>0.32623070856498299</v>
+        <v>0.39743771373710102</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="10" t="s">
-        <v>223</v>
+        <v>11</v>
       </c>
       <c r="B32" s="11">
-        <v>0.16274006457565099</v>
+        <v>0.198056698819602</v>
       </c>
       <c r="C32" s="11">
-        <v>3.6876426191857499E-2</v>
+        <v>2.8758871486911498E-3</v>
       </c>
       <c r="D32" s="11">
-        <v>0.32623070856498299</v>
+        <v>0.10321239433635999</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="10" t="s">
-        <v>250</v>
-      </c>
-      <c r="B33" s="11">
-        <v>0.17201846527610301</v>
-      </c>
-      <c r="C33" s="11">
-        <v>3.5586675930752001E-2</v>
-      </c>
-      <c r="D33" s="11">
-        <v>0.32623070856498299</v>
+      <c r="A33" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" s="15">
+        <v>0.21240903417253801</v>
+      </c>
+      <c r="C33" s="15">
+        <v>2.1006699903141401E-4</v>
+      </c>
+      <c r="D33" s="15">
+        <v>2.2617213562382301E-2</v>
       </c>
     </row>
     <row r="34" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
@@ -8332,27 +8332,27 @@
     </row>
     <row r="35" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="10" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="B35" s="11">
-        <v>0.28814801224839198</v>
+        <v>0.26198735124761902</v>
       </c>
       <c r="C35" s="11">
-        <v>3.49578428114267E-2</v>
+        <v>4.41947348085261E-2</v>
       </c>
       <c r="D35" s="11">
-        <v>0.32623070856498299</v>
+        <v>0.37565524587247101</v>
       </c>
     </row>
     <row r="36" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="10" t="s">
-        <v>231</v>
+        <v>160</v>
       </c>
       <c r="B36" s="11">
-        <v>0.28995857583905499</v>
+        <v>0.28814801224839198</v>
       </c>
       <c r="C36" s="11">
-        <v>2.4661731597025598E-2</v>
+        <v>3.49578428114267E-2</v>
       </c>
       <c r="D36" s="11">
         <v>0.32623070856498299</v>
@@ -8360,13 +8360,13 @@
     </row>
     <row r="37" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="10" t="s">
-        <v>131</v>
+        <v>231</v>
       </c>
       <c r="B37" s="11">
-        <v>0.556265463586193</v>
+        <v>0.28995857583905499</v>
       </c>
       <c r="C37" s="11">
-        <v>3.7370081166886601E-2</v>
+        <v>2.4661731597025598E-2</v>
       </c>
       <c r="D37" s="11">
         <v>0.32623070856498299</v>
@@ -8374,58 +8374,58 @@
     </row>
     <row r="38" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="10" t="s">
-        <v>181</v>
+        <v>130</v>
       </c>
       <c r="B38" s="11">
-        <v>0.86676358942383702</v>
+        <v>0.40876233409423801</v>
       </c>
       <c r="C38" s="11">
-        <v>3.6123796233079201E-2</v>
+        <v>7.2453229715699098E-3</v>
       </c>
       <c r="D38" s="11">
-        <v>0.32623070856498299</v>
+        <v>0.157671563728815</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="10" t="s">
-        <v>60</v>
+        <v>131</v>
       </c>
       <c r="B39" s="11">
-        <v>0.26198735124761902</v>
+        <v>0.556265463586193</v>
       </c>
       <c r="C39" s="11">
-        <v>4.41947348085261E-2</v>
+        <v>3.7370081166886601E-2</v>
       </c>
       <c r="D39" s="11">
-        <v>0.37565524587247101</v>
+        <v>0.32623070856498299</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B40" s="8">
-        <v>-0.42477578132881899</v>
-      </c>
-      <c r="C40" s="8">
-        <v>4.8658691314383697E-2</v>
-      </c>
-      <c r="D40" s="8">
-        <v>0.39743771373710102</v>
+      <c r="A40" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" s="11">
+        <v>0.60368195934063695</v>
+      </c>
+      <c r="C40" s="11">
+        <v>3.28809754458113E-3</v>
+      </c>
+      <c r="D40" s="11">
+        <v>0.10620555068997101</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="10" t="s">
-        <v>247</v>
+        <v>181</v>
       </c>
       <c r="B41" s="11">
-        <v>0.18582779031259</v>
+        <v>0.86676358942383702</v>
       </c>
       <c r="C41" s="11">
-        <v>4.9218292722860803E-2</v>
+        <v>3.6123796233079201E-2</v>
       </c>
       <c r="D41" s="11">
-        <v>0.39743771373710102</v>
+        <v>0.32623070856498299</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
@@ -9283,7 +9283,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D324">
-    <sortCondition ref="D1"/>
+    <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>